<commit_message>
changes to excel and transaction.py
</commit_message>
<xml_diff>
--- a/data/income.xlsx
+++ b/data/income.xlsx
@@ -1,27 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c1c741db71da0312/Desktop/VS Code Github/python-project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{B529CC69-1C7F-4C20-92B6-62554AAA3AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7B9D76C-BDD2-4F42-A35F-6118A6F5363F}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_2B59D2BFD3B058C38C891FD04BFD68B47803FF52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DCE435D-CD34-4CFA-A198-E66B90612195}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
+    <t>income_id</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>transaction_id</t>
+  </si>
+  <si>
     <t>Salary</t>
   </si>
   <si>
@@ -47,30 +65,15 @@
   </si>
   <si>
     <t>Graphic Design for SAF</t>
-  </si>
-  <si>
-    <t>income_id</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>transaction_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -125,7 +128,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,47 +434,46 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
-        <f>1</f>
         <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>45658</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>2500</v>
@@ -482,17 +484,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
-        <f xml:space="preserve"> A2 + 1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>45767</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>1000</v>
@@ -503,17 +504,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
-        <f t="shared" ref="A4:A12" si="0" xml:space="preserve"> A3 + 1</f>
         <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>45688</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>102.2</v>
@@ -524,17 +524,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>45689</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <v>2500</v>
@@ -545,17 +544,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="2">
         <v>45702</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E6">
         <v>288</v>
@@ -566,17 +564,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="2">
         <v>45716</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E7">
         <v>58.7</v>
@@ -587,17 +584,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
-        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="2">
         <v>45717</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E8">
         <v>2500</v>
@@ -608,17 +604,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="2">
         <v>45747</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E9">
         <v>17.010000000000002</v>
@@ -629,17 +624,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="2">
         <v>45748</v>
       </c>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E10">
         <v>2500</v>
@@ -650,17 +644,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="2">
         <v>45767</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E11">
         <v>1000</v>
@@ -671,17 +664,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
-        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="2">
         <v>45777</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E12">
         <v>45.67</v>

</xml_diff>